<commit_message>
add locks for lt cancel and update report
</commit_message>
<xml_diff>
--- a/excel_reports/Aaron_Butler.xlsx
+++ b/excel_reports/Aaron_Butler.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7760" uniqueCount="1879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7763" uniqueCount="1882">
   <si>
     <t>Policy Record</t>
   </si>
@@ -5582,10 +5582,13 @@
     <t>Current Month Active</t>
   </si>
   <si>
-    <t>Lifetime Cancels (12+ Month Duration)</t>
-  </si>
-  <si>
-    <t>(These plans are added back into Current Month Total Active)</t>
+    <t>Past Lifetime Cancels (12+ Month Duration)</t>
+  </si>
+  <si>
+    <t>Current Lifetime Cancels (12+ Month Duration)</t>
+  </si>
+  <si>
+    <t>(Any new long-term cancels are added back into Current Month Total Active)</t>
   </si>
   <si>
     <t>Net New Active</t>
@@ -5627,13 +5630,16 @@
     <t>Ancillary Plans</t>
   </si>
   <si>
-    <t>Previous Active DVH Plans:</t>
+    <t>Past Active DVH Plans:</t>
   </si>
   <si>
     <t>Current Active DVH Plans:</t>
   </si>
   <si>
-    <t>DVH Lifetime Cancels (12+ Month Duration)</t>
+    <t>Previous DVH Lifetime Cancels (12+ Month Duration)</t>
+  </si>
+  <si>
+    <t>Current DVH Lifetime Cancels (12+ Month Duration)</t>
   </si>
   <si>
     <t>Net New DVH Plans:</t>
@@ -5648,7 +5654,10 @@
     <t>Current Active Copay Plans:</t>
   </si>
   <si>
-    <t>Copay Lifetime Cancels (12+ Month Duration)</t>
+    <t>Past Copay Lifetime Cancels (12+ Month Duration)</t>
+  </si>
+  <si>
+    <t>Current Copay Lifetime Cancels (12+ Month Duration)</t>
   </si>
   <si>
     <t>Net New Copay Plans:</t>
@@ -6058,7 +6067,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6096,25 +6105,25 @@
       <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
         <v>1854</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>1855</v>
       </c>
-      <c r="B5" s="4">
-        <f>B3+B4-B2</f>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B6" s="4">
+        <f>-B2+B3-B4+B5</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>1856</v>
-      </c>
-      <c r="B6" s="2">
-        <v>-30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6122,62 +6131,70 @@
         <v>1857</v>
       </c>
       <c r="B7" s="2">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B8" s="2">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1858</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>1859</v>
-      </c>
-      <c r="B8" s="4">
-        <f>SUM(B5:B7)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>1860</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B9" s="4">
+        <f>SUM(B6:B8)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>1861</v>
       </c>
-      <c r="B9" s="5">
-        <f>MAX(0, B8*150)</f>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B10" s="5">
+        <f>MAX(0, B9*150)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>1862</v>
-      </c>
-    </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>1863</v>
       </c>
-      <c r="B12" s="2">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B13" s="2">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1878</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="B17" s="5">
         <f>SUM(Core!T:T)</f>
@@ -6186,12 +6203,12 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="B20">
         <v>38</v>
@@ -6199,7 +6216,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
       <c r="B21">
         <v>38</v>
@@ -6207,7 +6224,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -6215,25 +6232,33 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>1871</v>
-      </c>
-      <c r="B23">
-        <f>-B20+B21+B22</f>
+        <v>1872</v>
+      </c>
+      <c r="B23" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="4" t="s">
-        <v>1872</v>
-      </c>
-      <c r="B24" s="5">
-        <f>B23*50</f>
+      <c r="A24" s="2" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B24">
+        <f>-B20+B21-B22+B23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B25" s="5">
+        <f>B24*50</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>1873</v>
+        <v>1875</v>
       </c>
       <c r="B26">
         <v>9</v>
@@ -6241,7 +6266,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>1874</v>
+        <v>1876</v>
       </c>
       <c r="B27">
         <v>9</v>
@@ -6249,7 +6274,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>1875</v>
+        <v>1877</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -6257,19 +6282,27 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>1876</v>
-      </c>
-      <c r="B29">
-        <f>-B26+B27+B28</f>
+        <v>1878</v>
+      </c>
+      <c r="B29" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="4" t="s">
-        <v>1877</v>
-      </c>
-      <c r="B30" s="5">
-        <f>B29*100</f>
+      <c r="A30" s="2" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B30">
+        <f>-B26+B27-B28+B29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B31" s="5">
+        <f>B30*100</f>
         <v>0</v>
       </c>
     </row>
@@ -9923,7 +9956,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="13.7109375" style="8" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" style="8" customWidth="1"/>
     <col min="3" max="9" width="9.7109375" style="8" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" style="8" customWidth="1"/>
     <col min="11" max="16" width="11.7109375" customWidth="1"/>
@@ -29569,7 +29602,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="13.7109375" style="8" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" style="8" customWidth="1"/>
     <col min="3" max="9" width="9.7109375" style="8" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" style="8" customWidth="1"/>
     <col min="11" max="16" width="11.7109375" customWidth="1"/>
@@ -31477,7 +31510,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="13.7109375" style="8" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" style="8" customWidth="1"/>
     <col min="3" max="9" width="9.7109375" style="8" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" style="8" customWidth="1"/>
     <col min="11" max="16" width="11.7109375" customWidth="1"/>

</xml_diff>